<commit_message>
Set non-Kyoto gas GWP values to 0
</commit_message>
<xml_diff>
--- a/InputData/fuels/GbPbT/GWP by Pollutant by Timeframe.xlsx
+++ b/InputData/fuels/GbPbT/GWP by Pollutant by Timeframe.xlsx
@@ -1,27 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipL\InputData\fuels\GbPbT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\fuels\GbPbT\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2507C16-8FFD-4A24-9319-9C8A1575EA54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="135" windowWidth="24915" windowHeight="12330"/>
+    <workbookView xWindow="29895" yWindow="4140" windowWidth="26325" windowHeight="17235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="Data" sheetId="3" r:id="rId2"/>
     <sheet name="GbPbT" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
   <si>
     <t>Source:</t>
   </si>
@@ -104,24 +118,12 @@
     <t>Note</t>
   </si>
   <si>
-    <t>GWP values for VOC, CO, and NOx vary by region.  These values should</t>
-  </si>
-  <si>
-    <t>if creating a version of the model for another country.</t>
-  </si>
-  <si>
-    <t>be updated (likely from the same IPCC source, using different rows in the table)</t>
-  </si>
-  <si>
     <t>p. 740, Table 8.A.6, Row 2 (BC four regions)</t>
   </si>
   <si>
     <t>p. 740, Table 8.A.6, Row 7 (OC four regions)</t>
   </si>
   <si>
-    <t>BC and OC values only include aerosol-radiation interaction.</t>
-  </si>
-  <si>
     <t>100-Year GWP</t>
   </si>
   <si>
@@ -147,12 +149,15 @@
   </si>
   <si>
     <t>Global Warming Potential (g CO2e/g pollutant)</t>
+  </si>
+  <si>
+    <t>We use GWPs for the Kyoto gases (CO2, CH4, N2O, and F-gases)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -245,9 +250,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -285,9 +290,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -322,7 +327,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -357,7 +362,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -530,23 +535,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.1328125" customWidth="1"/>
-    <col min="3" max="3" width="41.3984375" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" customWidth="1"/>
+    <col min="3" max="3" width="41.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -554,54 +561,39 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
         <v>2013</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1"/>
+    <hyperlink ref="B6" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
@@ -609,32 +601,32 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="B11:D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="18.59765625" customWidth="1"/>
+    <col min="2" max="3" width="18.5703125" customWidth="1"/>
     <col min="4" max="4" width="80" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="5"/>
       <c r="B1" s="6" t="s">
         <v>12</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -648,7 +640,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -662,7 +654,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -676,7 +668,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -690,7 +682,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -701,10 +693,10 @@
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -715,10 +707,10 @@
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -729,10 +721,10 @@
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -743,10 +735,10 @@
         <v>345</v>
       </c>
       <c r="D9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -757,10 +749,10 @@
         <v>-46</v>
       </c>
       <c r="D10" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -774,7 +766,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -788,7 +780,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -802,12 +794,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
         <v>20</v>
       </c>
@@ -818,33 +810,35 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.3984375" customWidth="1"/>
-    <col min="2" max="2" width="17.3984375" customWidth="1"/>
-    <col min="3" max="3" width="20.265625" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="str">
         <f>Data!A2</f>
         <v>CO2</v>
@@ -858,119 +852,103 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="str">
         <f>Data!A3</f>
         <v>VOC</v>
       </c>
       <c r="B3" s="4">
-        <f>Data!B3</f>
-        <v>16.2</v>
+        <v>0</v>
       </c>
       <c r="C3" s="4">
-        <f>Data!C3</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="str">
         <f>Data!A4</f>
         <v>CO</v>
       </c>
       <c r="B4" s="4">
-        <f>Data!B4</f>
-        <v>5.6</v>
+        <v>0</v>
       </c>
       <c r="C4" s="4">
-        <f>Data!C4</f>
-        <v>1.8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="str">
         <f>Data!A5</f>
         <v>NOx</v>
       </c>
       <c r="B5" s="4">
-        <f>Data!B5</f>
-        <v>-2.4</v>
+        <v>0</v>
       </c>
       <c r="C5" s="4">
-        <f>Data!C5</f>
-        <v>-8.1999999999999993</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="str">
         <f>Data!A6</f>
         <v>PM10</v>
       </c>
       <c r="B6" s="4">
-        <f>Data!B6</f>
         <v>0</v>
       </c>
       <c r="C6" s="4">
-        <f>Data!C6</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="str">
         <f>Data!A7</f>
         <v>PM25</v>
       </c>
       <c r="B7" s="4">
-        <f>Data!B7</f>
         <v>0</v>
       </c>
       <c r="C7" s="4">
-        <f>Data!C7</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="str">
         <f>Data!A8</f>
         <v>SOx</v>
       </c>
       <c r="B8" s="4">
-        <f>Data!B8</f>
         <v>0</v>
       </c>
       <c r="C8" s="4">
-        <f>Data!C8</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="str">
         <f>Data!A9</f>
         <v>BC</v>
       </c>
       <c r="B9" s="4">
-        <f>Data!B9</f>
-        <v>1200</v>
+        <v>0</v>
       </c>
       <c r="C9" s="4">
-        <f>Data!C9</f>
-        <v>345</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="str">
         <f>Data!A10</f>
         <v>OC</v>
       </c>
       <c r="B10" s="4">
-        <f>Data!B10</f>
-        <v>-160</v>
+        <v>0</v>
       </c>
       <c r="C10" s="4">
-        <f>Data!C10</f>
-        <v>-46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="str">
         <f>Data!A11</f>
         <v>CH4</v>
@@ -984,7 +962,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="str">
         <f>Data!A12</f>
         <v>N2O</v>
@@ -998,7 +976,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="str">
         <f>Data!A13</f>
         <v>F gases</v>

</xml_diff>